<commit_message>
add cable & socket
</commit_message>
<xml_diff>
--- a/hardwareSpecification.xlsx
+++ b/hardwareSpecification.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="110">
   <x:si>
     <x:t>[SMG] 아두이노 대기압/고도 센서 모듈 BMP280 [TYE-BMP28]</x:t>
   </x:si>
@@ -64,6 +64,9 @@
     <x:t>https://www.devicemart.co.kr/goods/view?no=14486677</x:t>
   </x:si>
   <x:si>
+    <x:t>https://www.devicemart.co.kr/goods/view?no=3585</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.digikey.kr/ko/products/detail/stmicroelectronics/NUCLEO-F446RE/5347712</x:t>
   </x:si>
   <x:si>
@@ -139,6 +142,9 @@
     <x:t>보유</x:t>
   </x:si>
   <x:si>
+    <x:t>ETC</x:t>
+  </x:si>
+  <x:si>
     <x:t>NMEA0183</x:t>
   </x:si>
   <x:si>
@@ -323,13 +329,28 @@
   </x:si>
   <x:si>
     <x:t>Interface : UART / I2C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.devicemart.co.kr/goods/view?no=1321195</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[KEYES] 테스트[CH254] 소켓 점퍼 케이블 40P (칼라) (M/M) 20cm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[CONNFLY (중국)] 핀헤더소켓 Single 1x40 Straight(2.54mm)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.devicemart.co.kr/goods/view?no=1321196</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[KEYES] 테스트[CH254] 소켓 점퍼 케이블 40P (칼라) (M/F) 20cm</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="11">
+  <x:fonts count="12">
     <x:font>
       <x:name val="맑은 고딕"/>
       <x:sz val="11"/>
@@ -422,8 +443,33 @@
         </x:font>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:font hs:extension="1">
+          <x:name val="맑은 고딕"/>
+          <x:sz val="8"/>
+          <x:color rgb="ff0000ff"/>
+          <x:u/>
+          <hs:underlineShape val="solid"/>
+          <hs:underlineType val="1"/>
+          <hs:underlineColor rgb="ff0000ff"/>
+          <hs:size val="100"/>
+          <hs:ratio val="100"/>
+          <hs:spacing val="0"/>
+          <hs:offset val="0"/>
+        </x:font>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:font>
+          <x:name val="맑은 고딕"/>
+          <x:sz val="8"/>
+          <x:color rgb="ff0000ff"/>
+          <x:u/>
+        </x:font>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:fonts>
-  <x:fills count="8">
+  <x:fills count="9">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
@@ -466,6 +512,12 @@
         <x:bgColor auto="1"/>
       </x:patternFill>
     </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="ff9be5c8"/>
+        <x:bgColor auto="1"/>
+      </x:patternFill>
+    </x:fill>
   </x:fills>
   <x:borders count="1">
     <x:border diagonalUp="1" diagonalDown="1">
@@ -533,7 +585,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="30">
+  <x:cellXfs count="32">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -744,6 +796,22 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <x:alignment horizontal="general" vertical="center" wrapText="1"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="2">
     <x:cellStyle xfId="0" builtinId="0"/>
@@ -1544,10 +1612,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet3"/>
-  <x:dimension ref="B2:I56"/>
+  <x:dimension ref="B2:I60"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="K24" activeCellId="0" sqref="K24:K24"/>
+    <x:sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="G42" activeCellId="0" sqref="G42:G43"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9" defaultRowHeight="10.699999999999999"/>
@@ -1566,28 +1634,28 @@
     <x:row r="1" ht="14.1" customHeight="1"/>
     <x:row r="2" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B2" s="11" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C2" s="11" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D2" s="11" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="E2" s="11" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="F2" s="11" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="C2" s="11" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="D2" s="11" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="E2" s="11" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="F2" s="11" t="s">
-        <x:v>69</x:v>
-      </x:c>
       <x:c r="G2" s="11" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="H2" s="11" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="I2" s="11" t="s">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="2:9" ht="14.1" customHeight="1">
@@ -1602,20 +1670,20 @@
     </x:row>
     <x:row r="4" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B4" s="17" t="s">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C4" s="13" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D4" s="5" t="s">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="E4" s="13"/>
       <x:c r="F4" s="14">
         <x:v>278000</x:v>
       </x:c>
       <x:c r="G4" s="12" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="H4" s="13"/>
       <x:c r="I4" s="9">
@@ -1627,7 +1695,7 @@
       <x:c r="B5" s="17"/>
       <x:c r="C5" s="13"/>
       <x:c r="D5" s="5" t="s">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E5" s="13"/>
       <x:c r="F5" s="14"/>
@@ -1639,7 +1707,7 @@
       <x:c r="B6" s="17"/>
       <x:c r="C6" s="13"/>
       <x:c r="D6" s="5" t="s">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E6" s="13"/>
       <x:c r="F6" s="14"/>
@@ -1651,7 +1719,7 @@
       <x:c r="B7" s="17"/>
       <x:c r="C7" s="13"/>
       <x:c r="D7" s="4" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E7" s="13"/>
       <x:c r="F7" s="14"/>
@@ -1661,10 +1729,10 @@
     </x:row>
     <x:row r="8" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B8" s="26" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C8" s="20" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D8" s="4" t="s">
         <x:v>7</x:v>
@@ -1674,18 +1742,18 @@
         <x:v>14800</x:v>
       </x:c>
       <x:c r="G8" s="22" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H8" s="20"/>
       <x:c r="I8" s="23" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B9" s="26"/>
       <x:c r="C9" s="20"/>
       <x:c r="D9" s="4" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="E9" s="20"/>
       <x:c r="F9" s="21"/>
@@ -1697,7 +1765,7 @@
       <x:c r="B10" s="26"/>
       <x:c r="C10" s="20"/>
       <x:c r="D10" s="4" t="s">
-        <x:v>90</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="E10" s="20"/>
       <x:c r="F10" s="21"/>
@@ -1719,31 +1787,31 @@
     </x:row>
     <x:row r="12" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B12" s="27" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C12" s="20" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D12" s="4" t="s">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="E12" s="20"/>
       <x:c r="F12" s="21">
         <x:v>39800</x:v>
       </x:c>
       <x:c r="G12" s="22" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="H12" s="20"/>
       <x:c r="I12" s="25" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B13" s="27"/>
       <x:c r="C13" s="20"/>
       <x:c r="D13" s="4" t="s">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="E13" s="20"/>
       <x:c r="F13" s="21"/>
@@ -1755,7 +1823,7 @@
       <x:c r="B14" s="27"/>
       <x:c r="C14" s="20"/>
       <x:c r="D14" s="4" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="E14" s="20"/>
       <x:c r="F14" s="21"/>
@@ -1767,7 +1835,7 @@
       <x:c r="B15" s="27"/>
       <x:c r="C15" s="20"/>
       <x:c r="D15" s="4" t="s">
-        <x:v>81</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="E15" s="20"/>
       <x:c r="F15" s="21"/>
@@ -1779,7 +1847,7 @@
       <x:c r="B16" s="27"/>
       <x:c r="C16" s="20"/>
       <x:c r="D16" s="4" t="s">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E16" s="20"/>
       <x:c r="F16" s="21"/>
@@ -1791,7 +1859,7 @@
       <x:c r="B17" s="27"/>
       <x:c r="C17" s="20"/>
       <x:c r="D17" s="4" t="s">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="E17" s="20"/>
       <x:c r="F17" s="21"/>
@@ -1801,20 +1869,20 @@
     </x:row>
     <x:row r="18" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B18" s="28" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C18" s="20" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D18" s="4" t="s">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E18" s="20"/>
       <x:c r="F18" s="21">
         <x:v>85000</x:v>
       </x:c>
       <x:c r="G18" s="22" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="H18" s="20"/>
       <x:c r="I18" s="23">
@@ -1826,7 +1894,7 @@
       <x:c r="B19" s="28"/>
       <x:c r="C19" s="20"/>
       <x:c r="D19" s="4" t="s">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="E19" s="20"/>
       <x:c r="F19" s="21"/>
@@ -1838,7 +1906,7 @@
       <x:c r="B20" s="28"/>
       <x:c r="C20" s="20"/>
       <x:c r="D20" s="4" t="s">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="E20" s="20"/>
       <x:c r="F20" s="21"/>
@@ -1850,7 +1918,7 @@
       <x:c r="B21" s="28"/>
       <x:c r="C21" s="20"/>
       <x:c r="D21" s="4" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E21" s="20"/>
       <x:c r="F21" s="21"/>
@@ -1862,7 +1930,7 @@
       <x:c r="B22" s="28"/>
       <x:c r="C22" s="20"/>
       <x:c r="D22" s="4" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E22" s="20"/>
       <x:c r="F22" s="21"/>
@@ -1872,20 +1940,20 @@
     </x:row>
     <x:row r="23" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B23" s="19" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C23" s="13" t="s">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="D23" s="13" t="s">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="E23" s="13"/>
       <x:c r="F23" s="14">
         <x:v>22239</x:v>
       </x:c>
       <x:c r="G23" s="12" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H23" s="12" t="s">
         <x:v>13</x:v>
@@ -1907,10 +1975,10 @@
     </x:row>
     <x:row r="25" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B25" s="18" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C25" s="13" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D25" s="13" t="s">
         <x:v>6</x:v>
@@ -1920,7 +1988,7 @@
         <x:v>4730</x:v>
       </x:c>
       <x:c r="G25" s="12" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H25" s="13"/>
       <x:c r="I25" s="9">
@@ -1940,20 +2008,20 @@
     </x:row>
     <x:row r="27" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B27" s="17" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C27" s="13" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="D27" s="5" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="E27" s="13"/>
       <x:c r="F27" s="14">
         <x:v>2838</x:v>
       </x:c>
       <x:c r="G27" s="12" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="H27" s="13"/>
       <x:c r="I27" s="9">
@@ -1977,7 +2045,7 @@
       <x:c r="B29" s="17"/>
       <x:c r="C29" s="13"/>
       <x:c r="D29" s="5" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E29" s="13"/>
       <x:c r="F29" s="14"/>
@@ -1987,23 +2055,23 @@
     </x:row>
     <x:row r="30" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B30" s="16" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C30" s="13" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D30" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E30" s="13"/>
       <x:c r="F30" s="14">
         <x:v>17600</x:v>
       </x:c>
       <x:c r="G30" s="12" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="H30" s="12" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="I30" s="9">
         <x:f>F30</x:f>
@@ -2014,7 +2082,7 @@
       <x:c r="B31" s="16"/>
       <x:c r="C31" s="13"/>
       <x:c r="D31" s="5" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E31" s="13"/>
       <x:c r="F31" s="14"/>
@@ -2026,7 +2094,7 @@
       <x:c r="B32" s="16"/>
       <x:c r="C32" s="13"/>
       <x:c r="D32" s="5" t="s">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="E32" s="13"/>
       <x:c r="F32" s="14"/>
@@ -2038,7 +2106,7 @@
       <x:c r="B33" s="16"/>
       <x:c r="C33" s="13"/>
       <x:c r="D33" s="5" t="s">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="E33" s="13"/>
       <x:c r="F33" s="14"/>
@@ -2049,22 +2117,22 @@
     <x:row r="34" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B34" s="16"/>
       <x:c r="C34" s="13" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D34" s="5" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E34" s="13" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F34" s="14">
         <x:v>30800</x:v>
       </x:c>
       <x:c r="G34" s="12" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="H34" s="12" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="I34" s="9">
         <x:f>F34</x:f>
@@ -2087,7 +2155,7 @@
       <x:c r="B36" s="16"/>
       <x:c r="C36" s="13"/>
       <x:c r="D36" s="5" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E36" s="13"/>
       <x:c r="F36" s="14"/>
@@ -2108,10 +2176,10 @@
         <x:v>2200</x:v>
       </x:c>
       <x:c r="G37" s="12" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H37" s="12" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="I37" s="9">
         <x:f>F37</x:f>
@@ -2122,7 +2190,7 @@
       <x:c r="B38" s="16"/>
       <x:c r="C38" s="13"/>
       <x:c r="D38" s="5" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E38" s="13"/>
       <x:c r="F38" s="14"/>
@@ -2155,7 +2223,7 @@
         <x:v>5500</x:v>
       </x:c>
       <x:c r="G40" s="12" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="H40" s="13"/>
       <x:c r="I40" s="9">
@@ -2181,14 +2249,14 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D42" s="5" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="E42" s="13"/>
       <x:c r="F42" s="14">
         <x:v>1100</x:v>
       </x:c>
       <x:c r="G42" s="12" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="H42" s="13"/>
       <x:c r="I42" s="9">
@@ -2200,7 +2268,7 @@
       <x:c r="B43" s="16"/>
       <x:c r="C43" s="13"/>
       <x:c r="D43" s="5" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E43" s="13"/>
       <x:c r="F43" s="14"/>
@@ -2211,17 +2279,17 @@
     <x:row r="44" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B44" s="16"/>
       <x:c r="C44" s="13" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D44" s="5" t="s">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="E44" s="13"/>
       <x:c r="F44" s="14">
         <x:v>7700</x:v>
       </x:c>
       <x:c r="G44" s="12" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="H44" s="13"/>
       <x:c r="I44" s="9">
@@ -2233,7 +2301,7 @@
       <x:c r="B45" s="16"/>
       <x:c r="C45" s="13"/>
       <x:c r="D45" s="4" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E45" s="13"/>
       <x:c r="F45" s="14"/>
@@ -2244,10 +2312,10 @@
     <x:row r="46" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B46" s="29"/>
       <x:c r="C46" s="20" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D46" s="4" t="s">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="E46" s="4"/>
       <x:c r="F46" s="21">
@@ -2286,20 +2354,20 @@
     </x:row>
     <x:row r="49" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B49" s="15" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C49" s="13" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D49" s="4" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="E49" s="13"/>
       <x:c r="F49" s="14">
         <x:v>22000</x:v>
       </x:c>
       <x:c r="G49" s="12" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H49" s="13"/>
       <x:c r="I49" s="9">
@@ -2322,37 +2390,37 @@
     <x:row r="51" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B51" s="15"/>
       <x:c r="C51" s="5" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D51" s="5" t="s">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="E51" s="5"/>
       <x:c r="F51" s="6">
         <x:v>25300</x:v>
       </x:c>
       <x:c r="G51" s="7" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="H51" s="5"/>
       <x:c r="I51" s="8" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="2:9" ht="14.1" customHeight="1">
       <x:c r="B52" s="15"/>
       <x:c r="C52" s="13" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D52" s="5" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E52" s="13"/>
       <x:c r="F52" s="14">
         <x:v>8580</x:v>
       </x:c>
       <x:c r="G52" s="12" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H52" s="12" t="s">
         <x:v>12</x:v>
@@ -2366,7 +2434,7 @@
       <x:c r="B53" s="15"/>
       <x:c r="C53" s="13"/>
       <x:c r="D53" s="5" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E53" s="13"/>
       <x:c r="F53" s="14"/>
@@ -2380,30 +2448,98 @@
       <x:c r="D54" s="5"/>
       <x:c r="E54" s="5"/>
       <x:c r="F54" s="5"/>
-      <x:c r="G54" s="5"/>
+      <x:c r="G54" s="4"/>
       <x:c r="H54" s="5"/>
     </x:row>
-    <x:row r="55" spans="2:9">
-      <x:c r="B55" s="11"/>
-      <x:c r="C55" s="13"/>
-      <x:c r="D55" s="13"/>
-      <x:c r="E55" s="13"/>
-      <x:c r="F55" s="14"/>
-      <x:c r="G55" s="13"/>
-      <x:c r="H55" s="13"/>
-      <x:c r="I55" s="8">
+    <x:row r="55" spans="2:9" ht="14.1" customHeight="1">
+      <x:c r="B55" s="30" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C55" s="4" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="D55" s="4"/>
+      <x:c r="E55" s="4"/>
+      <x:c r="F55" s="4">
+        <x:v>528</x:v>
+      </x:c>
+      <x:c r="G55" s="31" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H55" s="4"/>
+      <x:c r="I55" s="2">
+        <x:f>F55</x:f>
+        <x:v>528</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="2:9" ht="14.1" customHeight="1">
+      <x:c r="B56" s="30"/>
+      <x:c r="C56" s="4" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="D56" s="4"/>
+      <x:c r="E56" s="4"/>
+      <x:c r="F56" s="4">
+        <x:v>935</x:v>
+      </x:c>
+      <x:c r="G56" s="31" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="H56" s="4"/>
+      <x:c r="I56" s="2">
+        <x:f>F56</x:f>
+        <x:v>935</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="2:9" ht="14.1" customHeight="1">
+      <x:c r="B57" s="30"/>
+      <x:c r="C57" s="4" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="D57" s="4"/>
+      <x:c r="E57" s="4"/>
+      <x:c r="F57" s="4">
+        <x:v>935</x:v>
+      </x:c>
+      <x:c r="G57" s="31" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="H57" s="4"/>
+      <x:c r="I57" s="2">
+        <x:f>F57</x:f>
+        <x:v>935</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="2:8" ht="14.1" customHeight="1">
+      <x:c r="B58" s="30"/>
+      <x:c r="C58" s="4"/>
+      <x:c r="D58" s="4"/>
+      <x:c r="E58" s="4"/>
+      <x:c r="F58" s="4"/>
+      <x:c r="G58" s="4"/>
+      <x:c r="H58" s="4"/>
+    </x:row>
+    <x:row r="59" spans="2:9">
+      <x:c r="B59" s="11"/>
+      <x:c r="C59" s="13"/>
+      <x:c r="D59" s="13"/>
+      <x:c r="E59" s="13"/>
+      <x:c r="F59" s="14"/>
+      <x:c r="G59" s="13"/>
+      <x:c r="H59" s="13"/>
+      <x:c r="I59" s="8">
         <x:f>SUM(I4:I53)</x:f>
         <x:v>554345</x:v>
       </x:c>
     </x:row>
-    <x:row r="56" spans="2:8">
-      <x:c r="B56" s="11"/>
-      <x:c r="C56" s="13"/>
-      <x:c r="D56" s="13"/>
-      <x:c r="E56" s="13"/>
-      <x:c r="F56" s="13"/>
-      <x:c r="G56" s="13"/>
-      <x:c r="H56" s="13"/>
+    <x:row r="60" spans="2:8">
+      <x:c r="B60" s="11"/>
+      <x:c r="C60" s="13"/>
+      <x:c r="D60" s="13"/>
+      <x:c r="E60" s="13"/>
+      <x:c r="F60" s="13"/>
+      <x:c r="G60" s="13"/>
+      <x:c r="H60" s="13"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="126">
@@ -2422,13 +2558,13 @@
     <x:mergeCell ref="I23:I24"/>
     <x:mergeCell ref="G52:G53"/>
     <x:mergeCell ref="H52:H53"/>
-    <x:mergeCell ref="B55:B56"/>
-    <x:mergeCell ref="C55:C56"/>
-    <x:mergeCell ref="D55:D56"/>
-    <x:mergeCell ref="E55:E56"/>
-    <x:mergeCell ref="F55:F56"/>
-    <x:mergeCell ref="G55:G56"/>
-    <x:mergeCell ref="H55:H56"/>
+    <x:mergeCell ref="B59:B60"/>
+    <x:mergeCell ref="C59:C60"/>
+    <x:mergeCell ref="D59:D60"/>
+    <x:mergeCell ref="E59:E60"/>
+    <x:mergeCell ref="F59:F60"/>
+    <x:mergeCell ref="G59:G60"/>
+    <x:mergeCell ref="H59:H60"/>
     <x:mergeCell ref="B49:B54"/>
     <x:mergeCell ref="C49:C50"/>
     <x:mergeCell ref="E49:E50"/>
@@ -2556,6 +2692,9 @@
     <x:hyperlink ref="G18:G22" r:id="rId19"/>
     <x:hyperlink ref="G44:G44" r:id="rId20"/>
     <x:hyperlink ref="G49:G49" r:id="rId21"/>
+    <x:hyperlink ref="G55:G55" r:id="rId22"/>
+    <x:hyperlink ref="G56:G56" r:id="rId23"/>
+    <x:hyperlink ref="G57:G57" r:id="rId24"/>
   </x:hyperlinks>
   <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>